<commit_message>
Updated code for Create Account and Sign In page
</commit_message>
<xml_diff>
--- a/MyMojioWebsite/src/com/mojio/xls/Suite.xlsx
+++ b/MyMojioWebsite/src/com/mojio/xls/Suite.xlsx
@@ -26,18 +26,21 @@
     <t>Runmode</t>
   </si>
   <si>
-    <t>Create_Account</t>
+    <t>CreateAccount</t>
   </si>
   <si>
     <t>Done</t>
   </si>
   <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>SignIn</t>
+  </si>
+  <si>
     <t>N</t>
   </si>
   <si>
-    <t>SignIn</t>
-  </si>
-  <si>
     <t>Home_Page</t>
   </si>
   <si>
@@ -60,9 +63,6 @@
   </si>
   <si>
     <t>ClaimMojio</t>
-  </si>
-  <si>
-    <t>Y</t>
   </si>
   <si>
     <t>BillingInformation</t>
@@ -247,7 +247,7 @@
   <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="F24" activeCellId="0" pane="topLeft" sqref="F24"/>
+      <selection activeCell="F10" activeCellId="0" pane="topLeft" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -287,95 +287,95 @@
         <v>4</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="4">
       <c r="A4" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="5">
       <c r="A5" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="6">
       <c r="A6" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="7">
       <c r="A7" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="8">
       <c r="A8" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="9">
       <c r="A9" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="10">
       <c r="A10" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="11">
       <c r="A11" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="12">
@@ -386,7 +386,7 @@
         <v>17</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="13">
@@ -397,7 +397,7 @@
         <v>4</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="14">
@@ -408,7 +408,7 @@
         <v>20</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="15">
@@ -419,7 +419,7 @@
         <v>4</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="16">
@@ -430,7 +430,7 @@
         <v>4</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="17">
@@ -441,7 +441,7 @@
         <v>24</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="18">
@@ -452,7 +452,7 @@
         <v>4</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="19">
@@ -463,7 +463,7 @@
         <v>4</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="20">
@@ -474,7 +474,7 @@
         <v>4</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="21">
@@ -485,7 +485,7 @@
         <v>4</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="22">
@@ -496,7 +496,7 @@
         <v>30</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="23">
@@ -507,7 +507,7 @@
         <v>32</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="24">
@@ -518,7 +518,7 @@
         <v>4</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="25">
@@ -529,7 +529,7 @@
         <v>4</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="26">
@@ -540,7 +540,7 @@
         <v>4</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="27">
@@ -549,7 +549,7 @@
       </c>
       <c r="B27" s="2"/>
       <c r="C27" s="2" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Code for Sign In, Create Account and Left Hand Panel
</commit_message>
<xml_diff>
--- a/MyMojioWebsite/src/com/mojio/xls/Suite.xlsx
+++ b/MyMojioWebsite/src/com/mojio/xls/Suite.xlsx
@@ -32,28 +32,28 @@
     <t>Done</t>
   </si>
   <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>SignIn</t>
+  </si>
+  <si>
+    <t>Home_Page</t>
+  </si>
+  <si>
+    <t>MyProfile</t>
+  </si>
+  <si>
+    <t>Dashboard_Page</t>
+  </si>
+  <si>
+    <t>RightHandPanel</t>
+  </si>
+  <si>
+    <t>LeftHandPanel</t>
+  </si>
+  <si>
     <t>Y</t>
-  </si>
-  <si>
-    <t>SignIn</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>Home_Page</t>
-  </si>
-  <si>
-    <t>MyProfile</t>
-  </si>
-  <si>
-    <t>Dashboard_Page</t>
-  </si>
-  <si>
-    <t>RightHandPanel</t>
-  </si>
-  <si>
-    <t>LeftHandPanel</t>
   </si>
   <si>
     <t>MyVehicles</t>
@@ -247,7 +247,7 @@
   <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="F10" activeCellId="0" pane="topLeft" sqref="F10"/>
+      <selection activeCell="I10" activeCellId="0" pane="topLeft" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -287,62 +287,62 @@
         <v>4</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="4">
       <c r="A4" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="5">
       <c r="A5" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="6">
       <c r="A6" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="7">
       <c r="A7" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="8">
       <c r="A8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>7</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="9">
@@ -353,7 +353,7 @@
         <v>4</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="10">
@@ -364,7 +364,7 @@
         <v>4</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="11">
@@ -375,7 +375,7 @@
         <v>4</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="12">
@@ -386,7 +386,7 @@
         <v>17</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="13">
@@ -397,7 +397,7 @@
         <v>4</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="14">
@@ -408,7 +408,7 @@
         <v>20</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="15">
@@ -419,7 +419,7 @@
         <v>4</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="16">
@@ -430,7 +430,7 @@
         <v>4</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="17">
@@ -441,7 +441,7 @@
         <v>24</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="18">
@@ -452,7 +452,7 @@
         <v>4</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="19">
@@ -463,7 +463,7 @@
         <v>4</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="20">
@@ -474,7 +474,7 @@
         <v>4</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="21">
@@ -485,7 +485,7 @@
         <v>4</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="22">
@@ -496,7 +496,7 @@
         <v>30</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="23">
@@ -507,7 +507,7 @@
         <v>32</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="24">
@@ -518,7 +518,7 @@
         <v>4</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="25">
@@ -529,7 +529,7 @@
         <v>4</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="26">
@@ -540,7 +540,7 @@
         <v>4</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="27">
@@ -549,7 +549,7 @@
       </c>
       <c r="B27" s="2"/>
       <c r="C27" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Code changes to Dashboard, My Vehicles and Home Page
Code changes to Dashboard, My Vehicles and Home Page
</commit_message>
<xml_diff>
--- a/MyMojioWebsite/src/com/mojio/xls/Suite.xlsx
+++ b/MyMojioWebsite/src/com/mojio/xls/Suite.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="39">
   <si>
     <t>TSID</t>
   </si>
@@ -41,6 +41,9 @@
     <t>Home_Page</t>
   </si>
   <si>
+    <t>Y</t>
+  </si>
+  <si>
     <t>MyProfile</t>
   </si>
   <si>
@@ -54,9 +57,6 @@
   </si>
   <si>
     <t>MyVehicles</t>
-  </si>
-  <si>
-    <t>Y</t>
   </si>
   <si>
     <t>MyMojios</t>
@@ -253,7 +253,7 @@
   <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="C9" activeCellId="0" pane="topLeft" sqref="C9"/>
+      <selection activeCell="F11" activeCellId="0" pane="topLeft" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -302,12 +302,12 @@
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="5">
       <c r="A5" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
@@ -316,7 +316,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="6">
       <c r="A6" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>4</v>
@@ -327,7 +327,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="7">
       <c r="A7" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
@@ -336,7 +336,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="8">
       <c r="A8" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>4</v>
@@ -347,11 +347,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="9">
       <c r="A9" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="2"/>
+        <v>13</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C9" s="2" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="10">

</xml_diff>

<commit_message>
Code changes to Home suite
Code changes to Home suite
</commit_message>
<xml_diff>
--- a/MyMojioWebsite/src/com/mojio/xls/Suite.xlsx
+++ b/MyMojioWebsite/src/com/mojio/xls/Suite.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="38">
   <si>
     <t>TSID</t>
   </si>
@@ -41,30 +41,33 @@
     <t>Home_Page</t>
   </si>
   <si>
+    <t>MyProfile</t>
+  </si>
+  <si>
+    <t>Dashboard_Page</t>
+  </si>
+  <si>
+    <t>RightHandPanel</t>
+  </si>
+  <si>
+    <t>LeftHandPanel</t>
+  </si>
+  <si>
+    <t>MyVehicles</t>
+  </si>
+  <si>
+    <t>MyMojios</t>
+  </si>
+  <si>
+    <t>ClaimMojio</t>
+  </si>
+  <si>
+    <t>In Progress</t>
+  </si>
+  <si>
     <t>Y</t>
   </si>
   <si>
-    <t>MyProfile</t>
-  </si>
-  <si>
-    <t>Dashboard_Page</t>
-  </si>
-  <si>
-    <t>RightHandPanel</t>
-  </si>
-  <si>
-    <t>LeftHandPanel</t>
-  </si>
-  <si>
-    <t>MyVehicles</t>
-  </si>
-  <si>
-    <t>MyMojios</t>
-  </si>
-  <si>
-    <t>ClaimMojio</t>
-  </si>
-  <si>
     <t>BillingInformation</t>
   </si>
   <si>
@@ -89,13 +92,7 @@
     <t>LocateVehicle</t>
   </si>
   <si>
-    <t>In Progress</t>
-  </si>
-  <si>
     <t>TripHistory</t>
-  </si>
-  <si>
-    <t>Date search remains</t>
   </si>
   <si>
     <t>SendFeedback</t>
@@ -253,7 +250,7 @@
   <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="F11" activeCellId="0" pane="topLeft" sqref="F11"/>
+      <selection activeCell="A19" activeCellId="0" pane="topLeft" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -300,14 +297,16 @@
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="2"/>
+      <c r="B4" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C4" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="5">
       <c r="A5" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
@@ -316,7 +315,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="6">
       <c r="A6" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>4</v>
@@ -327,7 +326,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="7">
       <c r="A7" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
@@ -336,7 +335,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="8">
       <c r="A8" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>4</v>
@@ -347,7 +346,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="9">
       <c r="A9" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>4</v>
@@ -358,7 +357,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="10">
       <c r="A10" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2" t="s">
@@ -367,19 +366,21 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="11">
       <c r="A11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="2"/>
       <c r="C11" s="2" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="12">
       <c r="A12" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>5</v>
@@ -387,21 +388,19 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="13">
       <c r="A13" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>4</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="B13" s="2"/>
       <c r="C13" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="14">
       <c r="A14" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>5</v>
@@ -409,10 +408,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="15">
       <c r="A15" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>5</v>
@@ -420,10 +419,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="16">
       <c r="A16" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>5</v>
@@ -433,16 +432,14 @@
       <c r="A17" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>26</v>
-      </c>
+      <c r="B17" s="2"/>
       <c r="C17" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="18">
       <c r="A18" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="2" t="s">
@@ -451,7 +448,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="19">
       <c r="A19" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="2" t="s">
@@ -460,7 +457,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="20">
       <c r="A20" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="2" t="s">
@@ -469,7 +466,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="21">
       <c r="A21" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2" t="s">
@@ -478,10 +475,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="22">
       <c r="A22" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>32</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>5</v>
@@ -489,10 +486,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="23">
       <c r="A23" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>34</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>5</v>
@@ -500,7 +497,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="24">
       <c r="A24" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" s="2" t="s">
@@ -509,7 +506,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="25">
       <c r="A25" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="2" t="s">
@@ -518,7 +515,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="26">
       <c r="A26" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" s="2" t="s">
@@ -527,7 +524,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="27">
       <c r="A27" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" s="2" t="s">

</xml_diff>

<commit_message>
Added new code for FAQ module and updated code.
Added new code for FAQ module and updated code.
</commit_message>
<xml_diff>
--- a/MyMojioWebsite/src/com/mojio/xls/Suite.xlsx
+++ b/MyMojioWebsite/src/com/mojio/xls/Suite.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="39">
   <si>
     <t>TSID</t>
   </si>
@@ -71,31 +71,34 @@
     <t>Client stopped it</t>
   </si>
   <si>
+    <t>FAQ</t>
+  </si>
+  <si>
     <t>Contact_Support</t>
   </si>
   <si>
+    <t>MojioShop</t>
+  </si>
+  <si>
+    <t>Mojio Store-- not a part of My Mojio</t>
+  </si>
+  <si>
+    <t>MyOrders</t>
+  </si>
+  <si>
+    <t>My orders-- not a part of My Mojio</t>
+  </si>
+  <si>
+    <t>LocateVehicle</t>
+  </si>
+  <si>
+    <t>TripHistory</t>
+  </si>
+  <si>
+    <t>SendFeedback</t>
+  </si>
+  <si>
     <t>Y</t>
-  </si>
-  <si>
-    <t>MojioShop</t>
-  </si>
-  <si>
-    <t>Mojio Store-- not a part of My Mojio</t>
-  </si>
-  <si>
-    <t>MyOrders</t>
-  </si>
-  <si>
-    <t>My orders-- not a part of My Mojio</t>
-  </si>
-  <si>
-    <t>LocateVehicle</t>
-  </si>
-  <si>
-    <t>TripHistory</t>
-  </si>
-  <si>
-    <t>SendFeedback</t>
   </si>
   <si>
     <t>Settings</t>
@@ -247,10 +250,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="E13" activeCellId="0" pane="topLeft" sqref="E13"/>
+      <selection activeCell="C19" activeCellId="0" pane="topLeft" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -392,26 +395,24 @@
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="14">
       <c r="A14" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>21</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="B14" s="2"/>
       <c r="C14" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="15">
       <c r="A15" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>5</v>
@@ -419,10 +420,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="16">
       <c r="A16" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>5</v>
@@ -430,16 +431,18 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="17">
       <c r="A17" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B17" s="2"/>
+        <v>24</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="C17" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="18">
       <c r="A18" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="2" t="s">
@@ -448,11 +451,11 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="19">
       <c r="A19" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="2" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="20">
@@ -477,19 +480,17 @@
       <c r="A22" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>31</v>
-      </c>
+      <c r="B22" s="2"/>
       <c r="C22" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="23">
       <c r="A23" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>33</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>5</v>
@@ -497,9 +498,11 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="24">
       <c r="A24" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B24" s="2"/>
       <c r="C24" s="2" t="s">
         <v>5</v>
       </c>
@@ -528,6 +531,15 @@
       </c>
       <c r="B27" s="2"/>
       <c r="C27" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="28">
+      <c r="A28" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Code Commit 18 Feb 2015
Code changes to Admin Dashboard, Right Hand Panel and Settings
</commit_message>
<xml_diff>
--- a/MyMojioWebsite/src/com/mojio/xls/Suite.xlsx
+++ b/MyMojioWebsite/src/com/mojio/xls/Suite.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="38">
   <si>
     <t>TSID</t>
   </si>
@@ -62,9 +62,6 @@
     <t>ClaimMojio</t>
   </si>
   <si>
-    <t>In Progress</t>
-  </si>
-  <si>
     <t>BillingInformation</t>
   </si>
   <si>
@@ -98,16 +95,16 @@
     <t>SendFeedback</t>
   </si>
   <si>
+    <t>Settings</t>
+  </si>
+  <si>
+    <t>AdminSearch</t>
+  </si>
+  <si>
+    <t>AdminDashboard</t>
+  </si>
+  <si>
     <t>Y</t>
-  </si>
-  <si>
-    <t>Settings</t>
-  </si>
-  <si>
-    <t>AdminSearch</t>
-  </si>
-  <si>
-    <t>AdminDashboard</t>
   </si>
   <si>
     <t>ReplayEvent</t>
@@ -253,7 +250,7 @@
   <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="C19" activeCellId="0" pane="topLeft" sqref="C19"/>
+      <selection activeCell="G13" activeCellId="0" pane="topLeft" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -362,7 +359,9 @@
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="2"/>
+      <c r="B10" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C10" s="2" t="s">
         <v>5</v>
       </c>
@@ -372,7 +371,7 @@
         <v>14</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>5</v>
@@ -380,10 +379,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="12">
       <c r="A12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>17</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>5</v>
@@ -391,28 +390,32 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="13">
       <c r="A13" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" s="2"/>
+        <v>17</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C13" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="14">
       <c r="A14" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14" s="2"/>
+        <v>18</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C14" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="15">
       <c r="A15" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>21</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>5</v>
@@ -420,10 +423,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="16">
       <c r="A16" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>23</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>5</v>
@@ -431,10 +434,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="17">
       <c r="A17" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>5</v>
@@ -442,7 +445,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="18">
       <c r="A18" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="2" t="s">
@@ -451,16 +454,18 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="19">
       <c r="A19" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B19" s="2"/>
+        <v>25</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C19" s="2" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="20">
       <c r="A20" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="2" t="s">
@@ -469,7 +474,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="21">
       <c r="A21" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2" t="s">
@@ -478,19 +483,19 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="22">
       <c r="A22" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="2" t="s">
-        <v>5</v>
+        <v>29</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="23">
       <c r="A23" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>32</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>5</v>
@@ -498,10 +503,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="24">
       <c r="A24" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>34</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>5</v>
@@ -509,7 +514,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="25">
       <c r="A25" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="2" t="s">
@@ -518,7 +523,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="26">
       <c r="A26" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" s="2" t="s">
@@ -527,7 +532,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="27">
       <c r="A27" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" s="2" t="s">
@@ -536,7 +541,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="28">
       <c r="A28" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" s="2" t="s">

</xml_diff>